<commit_message>
updates thurs from @mac
</commit_message>
<xml_diff>
--- a/data/Glossary_SARA.xlsx
+++ b/data/Glossary_SARA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andres/Library/Mobile Documents/com~apple~CloudDocs/SARA-GFDRR/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA84CD8-D448-4C4D-9EBA-0E4F615E7BF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B5BB4A-4D45-B24F-8A18-E2A884F6FE2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-1680" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{F6C40C2E-E072-E94B-9B8F-C2523D257E0E}"/>
+    <workbookView xWindow="28800" yWindow="-1220" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{F6C40C2E-E072-E94B-9B8F-C2523D257E0E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tab Banners" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>This contains a summary of the GFDRR program overall, including an overview of the portfolio and donor contributions.</t>
   </si>
@@ -238,6 +238,16 @@
   </si>
   <si>
     <t>Combined Report (Master)</t>
+  </si>
+  <si>
+    <t>Pivot Table Report</t>
+  </si>
+  <si>
+    <t>The output of this report includes summary tables (pivot tables) for GFDRR's Porfolio by: 
+(1) GP/Global Theme &amp; Disbursment Risk Level; 
+(2) Trustee &amp; Disbursement Risk Level;
+(3) Country/Region and Disbursement Risk Level. 
+The report can be customized by selecting (using the buttons on the right) relevant categories to include (or not) in the report.  The report also provides a raw list of the grants used for the tables, for your reference.</t>
   </si>
 </sst>
 </file>
@@ -639,7 +649,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -706,10 +716,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DE94956-FF54-8442-B99C-3DD9A10D996C}">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="B33" sqref="B32:B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -942,6 +952,14 @@
         <v>60</v>
       </c>
     </row>
+    <row r="29" spans="1:2" ht="119" x14ac:dyDescent="0.2">
+      <c r="A29" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B24">
     <sortCondition ref="A2:A24"/>

</xml_diff>

<commit_message>
glossary and comms data update @PC
</commit_message>
<xml_diff>
--- a/data/Glossary_SARA.xlsx
+++ b/data/Glossary_SARA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andres/Library/Mobile Documents/com~apple~CloudDocs/SARA-GFDRR/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb480070\OneDrive - WBG\SARA-GFDRR\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B5BB4A-4D45-B24F-8A18-E2A884F6FE2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{F9B5BB4A-4D45-B24F-8A18-E2A884F6FE2A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{681A41A4-F8D9-4F91-A8A9-D99BB5D3F9C4}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-1220" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{F6C40C2E-E072-E94B-9B8F-C2523D257E0E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{F6C40C2E-E072-E94B-9B8F-C2523D257E0E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tab Banners" sheetId="1" r:id="rId1"/>
@@ -24,9 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>This contains a summary of the GFDRR program overall, including an overview of the portfolio and donor contributions.</t>
   </si>
@@ -248,6 +246,12 @@
 (2) Trustee &amp; Disbursement Risk Level;
 (3) Country/Region and Disbursement Risk Level. 
 The report can be customized by selecting (using the buttons on the right) relevant categories to include (or not) in the report.  The report also provides a raw list of the grants used for the tables, for your reference.</t>
+  </si>
+  <si>
+    <t>M&amp;E Platform Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Downloads raw data from GFDRR's M&amp;E Platform Portfolio Data List Tab. Notably, SARA populates the missing Funding Sources column prior to donwloading the data. </t>
   </si>
 </sst>
 </file>
@@ -652,13 +656,13 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.83203125" customWidth="1"/>
+    <col min="1" max="1" width="32.796875" customWidth="1"/>
     <col min="2" max="2" width="75.5" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -666,7 +670,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -674,7 +678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -682,7 +686,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -690,7 +694,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -698,7 +702,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>51</v>
       </c>
@@ -706,7 +710,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
     </row>
   </sheetData>
@@ -716,19 +720,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DE94956-FF54-8442-B99C-3DD9A10D996C}">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B33" sqref="B32:B33"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="39.5" customWidth="1"/>
-    <col min="2" max="2" width="111.1640625" customWidth="1"/>
+    <col min="2" max="2" width="111.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>54</v>
       </c>
@@ -736,7 +740,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -744,7 +748,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -752,7 +756,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -760,7 +764,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -768,7 +772,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -776,7 +780,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>36</v>
       </c>
@@ -784,7 +788,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>10</v>
       </c>
@@ -792,7 +796,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -800,7 +804,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -808,7 +812,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>47</v>
       </c>
@@ -816,7 +820,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>62</v>
       </c>
@@ -824,7 +828,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -832,7 +836,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -840,7 +844,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -848,7 +852,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -856,7 +860,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -864,7 +868,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" ht="37.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>40</v>
       </c>
@@ -872,7 +876,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -880,7 +884,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -888,7 +892,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>45</v>
       </c>
@@ -896,7 +900,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -904,7 +908,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>49</v>
       </c>
@@ -912,7 +916,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -920,7 +924,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
         <v>55</v>
       </c>
@@ -928,7 +932,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
         <v>56</v>
       </c>
@@ -936,7 +940,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>67</v>
       </c>
@@ -944,7 +948,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
         <v>61</v>
       </c>
@@ -952,12 +956,20 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="119" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" ht="111.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
         <v>68</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>